<commit_message>
Added extensive tests. Added some comments into parser file.
</commit_message>
<xml_diff>
--- a/tests/excel_files/test_fake_data_after_empty_column_x_before_444.xlsx
+++ b/tests/excel_files/test_fake_data_after_empty_column_x_before_444.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">random</t>
   </si>
@@ -44,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,8 +103,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -131,57 +135,57 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>44</v>
       </c>
     </row>
@@ -194,65 +198,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>111</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>222</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>333</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>444</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>